<commit_message>
added drop_columns to yaml config and data preprocess
</commit_message>
<xml_diff>
--- a/experiments/preprocessing/debug_splits/split_summary.xlsx
+++ b/experiments/preprocessing/debug_splits/split_summary.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3000</v>
+        <v>250</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>60.0%</t>
+          <t>59.8%</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>no: 90.40%, yes: 9.60%</t>
+          <t>no: 63.60%, yes: 36.40%</t>
         </is>
       </c>
     </row>
@@ -490,19 +490,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1000</v>
+        <v>84</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>20.1%</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>no: 90.40%, yes: 9.60%</t>
+          <t>no: 64.29%, yes: 35.71%</t>
         </is>
       </c>
     </row>
@@ -513,19 +513,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>84</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>20.0%</t>
+          <t>20.1%</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>no: 90.40%, yes: 9.60%</t>
+          <t>no: 63.10%, yes: 36.90%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
updated eval optimal recall threshold
</commit_message>
<xml_diff>
--- a/experiments/preprocessing/debug_splits/split_summary.xlsx
+++ b/experiments/preprocessing/debug_splits/split_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,22 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Target_Distribution</t>
+          <t>Target_Mean</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Target_Std</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Target_Min</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Target_Max</t>
         </is>
       </c>
     </row>
@@ -467,20 +482,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>250</v>
+        <v>534</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>59.8%</t>
+          <t>59.9%</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>276</v>
+        <v>532</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>no: 63.60%, yes: 36.40%</t>
-        </is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>0.49</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -490,20 +516,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>84</v>
+        <v>178</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20.1%</t>
+          <t>20.0%</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>78</v>
+        <v>169</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>no: 64.29%, yes: 35.71%</t>
-        </is>
+          <t>0.41</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.49</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -513,7 +550,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>84</v>
+        <v>179</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -521,12 +558,23 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>no: 63.10%, yes: 36.90%</t>
-        </is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>0.48</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>